<commit_message>
Add revisions of ch2
</commit_message>
<xml_diff>
--- a/final-reports/report/Images/Background/classification-opt.xlsx
+++ b/final-reports/report/Images/Background/classification-opt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KatB\Projects\Github\Thesis-report\MscThesis\final-reports\report\Images\Background\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catar\Projects\Research Projects\ThesisReport\MscThesis\final-reports\report\Images\Background\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:0_{6649F9A2-9322-45E9-BBB5-553D35AFB596}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{167A2219-AD0A-4B3B-8F2B-229D71E800DB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{2C5B380D-3C94-4C5A-BA57-F8B4E0B0BCE2}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="25440" windowHeight="15990" xr2:uid="{2C5B380D-3C94-4C5A-BA57-F8B4E0B0BCE2}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="23">
   <si>
     <t>Optimization</t>
   </si>
@@ -85,6 +85,21 @@
   </si>
   <si>
     <t>Algorithms</t>
+  </si>
+  <si>
+    <t>Optimization Problems</t>
+  </si>
+  <si>
+    <t>Optimization Algorithms</t>
+  </si>
+  <si>
+    <t>Determinism</t>
+  </si>
+  <si>
+    <t>Stochastic</t>
+  </si>
+  <si>
+    <t>Deterministic</t>
   </si>
 </sst>
 </file>
@@ -238,18 +253,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -261,41 +270,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -315,7 +339,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -611,354 +635,558 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52183C07-4D10-40ED-9BFD-6616E1AFB62E}">
-  <dimension ref="B3:AB36"/>
+  <dimension ref="B3:AF49"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D17" workbookViewId="0">
-      <selection activeCell="P36" sqref="P36"/>
+    <sheetView tabSelected="1" topLeftCell="G32" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
+      <selection activeCell="U38" sqref="U38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.83984375" style="3"/>
-    <col min="2" max="2" width="11.83984375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="0.62890625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="10" style="7" customWidth="1"/>
-    <col min="5" max="5" width="0.62890625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10.83984375" style="7" customWidth="1"/>
-    <col min="7" max="7" width="0.62890625" style="3" customWidth="1"/>
-    <col min="8" max="8" width="13.9453125" style="7" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="0.62890625" style="3" customWidth="1"/>
-    <col min="10" max="10" width="9.578125" style="3" customWidth="1"/>
-    <col min="11" max="11" width="2.578125" style="3" customWidth="1"/>
-    <col min="12" max="12" width="9.578125" style="3" customWidth="1"/>
-    <col min="13" max="13" width="4.578125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="5.1015625" style="3" customWidth="1"/>
-    <col min="15" max="15" width="2.578125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="5.1015625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="4.578125" style="3" customWidth="1"/>
-    <col min="18" max="18" width="11.578125" style="3" customWidth="1"/>
-    <col min="19" max="19" width="2.578125" style="3" customWidth="1"/>
-    <col min="20" max="20" width="11.578125" style="3" customWidth="1"/>
-    <col min="21" max="21" width="4.578125" style="3" customWidth="1"/>
-    <col min="22" max="22" width="14.1015625" style="3" customWidth="1"/>
-    <col min="23" max="23" width="2.578125" style="3" customWidth="1"/>
-    <col min="24" max="24" width="14.1015625" style="3" customWidth="1"/>
-    <col min="25" max="25" width="4.578125" style="3" customWidth="1"/>
-    <col min="26" max="26" width="5.578125" style="3" customWidth="1"/>
-    <col min="27" max="27" width="2.578125" style="3" customWidth="1"/>
-    <col min="28" max="28" width="5.578125" style="3" customWidth="1"/>
-    <col min="29" max="16384" width="8.83984375" style="3"/>
+    <col min="1" max="1" width="8.85546875" style="2"/>
+    <col min="2" max="2" width="11.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="0.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10" style="5" customWidth="1"/>
+    <col min="5" max="5" width="0.5703125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="5" customWidth="1"/>
+    <col min="7" max="8" width="0.5703125" style="2" customWidth="1"/>
+    <col min="9" max="9" width="1.7109375" style="5" customWidth="1"/>
+    <col min="10" max="13" width="5.28515625" style="2" customWidth="1"/>
+    <col min="14" max="17" width="4.7109375" style="2" customWidth="1"/>
+    <col min="18" max="19" width="5.7109375" style="2" customWidth="1"/>
+    <col min="20" max="20" width="4.7109375" style="2" customWidth="1"/>
+    <col min="21" max="24" width="8.7109375" style="2" customWidth="1"/>
+    <col min="25" max="28" width="4.7109375" style="2" customWidth="1"/>
+    <col min="29" max="32" width="6.7109375" style="2" customWidth="1"/>
+    <col min="33" max="33" width="1.85546875" style="2" customWidth="1"/>
+    <col min="34" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="D3" s="2"/>
-      <c r="F3" s="3"/>
-      <c r="H3" s="2"/>
-      <c r="J3" s="7"/>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="J4" s="7"/>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B5" s="4" t="s">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="D3" s="1"/>
+      <c r="F3" s="2"/>
+      <c r="I3" s="1"/>
+      <c r="K3" s="5"/>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="K4" s="5"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="11" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E5" s="9"/>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="6"/>
+      <c r="F5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="7" t="s">
+      <c r="G5" s="4"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="7"/>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B6" s="4"/>
-      <c r="D6" s="11"/>
-      <c r="F6" s="8"/>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B7" s="4"/>
-      <c r="D7" s="11"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="7" t="s">
+      <c r="K5" s="5"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="21"/>
+      <c r="D6" s="20"/>
+      <c r="F6" s="22"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="21"/>
+      <c r="D7" s="20"/>
+      <c r="F7" s="22"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B8" s="4"/>
-      <c r="D8" s="11"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B9" s="4"/>
-      <c r="D9" s="11"/>
-      <c r="F9" s="8" t="s">
+    <row r="8" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B8" s="21"/>
+      <c r="D8" s="20"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B9" s="21"/>
+      <c r="D9" s="20"/>
+      <c r="F9" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="7" t="s">
+      <c r="G9" s="4"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B10" s="4"/>
-      <c r="D10" s="11"/>
-      <c r="F10" s="8"/>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B11" s="4"/>
-      <c r="D11" s="11"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="7" t="s">
+    <row r="10" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B10" s="21"/>
+      <c r="D10" s="20"/>
+      <c r="F10" s="22"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B11" s="21"/>
+      <c r="D11" s="20"/>
+      <c r="F11" s="22"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B12" s="4"/>
-      <c r="D12" s="11"/>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B13" s="4"/>
-      <c r="D13" s="11"/>
-      <c r="F13" s="8" t="s">
+    <row r="12" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B12" s="21"/>
+      <c r="D12" s="20"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="21"/>
+      <c r="D13" s="20"/>
+      <c r="F13" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="6"/>
-      <c r="H13" s="7" t="s">
+      <c r="G13" s="4"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B14" s="4"/>
-      <c r="D14" s="11"/>
-      <c r="F14" s="8"/>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B15" s="4"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="10"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="7" t="s">
+    <row r="14" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="21"/>
+      <c r="D14" s="20"/>
+      <c r="F14" s="22"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B15" s="21"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="7"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="14"/>
+      <c r="I15" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.55000000000000004">
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="2:28" x14ac:dyDescent="0.55000000000000004">
-      <c r="B17" s="4"/>
-      <c r="D17" s="8" t="s">
+    <row r="16" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B16" s="21"/>
+    </row>
+    <row r="17" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B17" s="21"/>
+      <c r="D17" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F17" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G17" s="6"/>
-      <c r="H17" s="7" t="s">
+      <c r="G17" s="4"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="2:28" x14ac:dyDescent="0.55000000000000004">
-      <c r="B18" s="4"/>
-      <c r="D18" s="8"/>
-      <c r="F18" s="8"/>
-    </row>
-    <row r="19" spans="2:28" x14ac:dyDescent="0.55000000000000004">
-      <c r="B19" s="4"/>
-      <c r="D19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="7" t="s">
+    <row r="18" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B18" s="21"/>
+      <c r="D18" s="22"/>
+      <c r="F18" s="22"/>
+    </row>
+    <row r="19" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B19" s="21"/>
+      <c r="D19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="2:28" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="4"/>
-      <c r="D20" s="8"/>
-    </row>
-    <row r="21" spans="2:28" x14ac:dyDescent="0.55000000000000004">
-      <c r="B21" s="4"/>
-      <c r="D21" s="8"/>
-      <c r="F21" s="8" t="s">
+    <row r="20" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B20" s="21"/>
+      <c r="D20" s="22"/>
+    </row>
+    <row r="21" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B21" s="21"/>
+      <c r="D21" s="22"/>
+      <c r="F21" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="G21" s="6"/>
-      <c r="H21" s="7" t="s">
+      <c r="G21" s="4"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="2:28" x14ac:dyDescent="0.55000000000000004">
-      <c r="B22" s="4"/>
-      <c r="D22" s="8"/>
-      <c r="F22" s="8"/>
-    </row>
-    <row r="23" spans="2:28" x14ac:dyDescent="0.55000000000000004">
-      <c r="B23" s="4"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="7" t="s">
+    <row r="22" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B22" s="21"/>
+      <c r="D22" s="22"/>
+      <c r="F22" s="22"/>
+    </row>
+    <row r="23" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B23" s="21"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="14"/>
+      <c r="I23" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="26" spans="2:28" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
-      <c r="N26" s="1" t="s">
+    <row r="26" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="O26" s="13"/>
-      <c r="P26" s="13"/>
-      <c r="Q26" s="13"/>
-      <c r="R26" s="13"/>
-      <c r="S26" s="13"/>
-      <c r="T26" s="13"/>
-      <c r="U26" s="13"/>
-      <c r="V26" s="13"/>
-      <c r="W26" s="13"/>
-      <c r="X26" s="13"/>
-      <c r="Y26" s="2"/>
-      <c r="Z26" s="2"/>
-      <c r="AA26" s="2"/>
-      <c r="AB26" s="2"/>
-    </row>
-    <row r="27" spans="2:28" ht="6.3" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="N27" s="18"/>
-      <c r="O27" s="16"/>
-      <c r="X27" s="15"/>
-    </row>
-    <row r="28" spans="2:28" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="K28" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="L28" s="13"/>
-      <c r="M28" s="13"/>
-      <c r="N28" s="13"/>
-      <c r="O28" s="13"/>
-      <c r="P28" s="13"/>
-      <c r="Q28" s="13"/>
-      <c r="R28" s="13"/>
-      <c r="S28" s="2"/>
-      <c r="T28" s="2"/>
-      <c r="W28" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="X28" s="13"/>
-      <c r="Y28" s="13"/>
-      <c r="Z28" s="13"/>
-      <c r="AA28" s="2"/>
-      <c r="AB28" s="2"/>
-    </row>
-    <row r="29" spans="2:28" ht="6.9" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="J29" s="18"/>
-      <c r="K29" s="16"/>
-      <c r="O29" s="16"/>
-      <c r="S29" s="17"/>
-      <c r="W29" s="17"/>
-      <c r="AA29" s="17"/>
-    </row>
-    <row r="30" spans="2:28" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="J30" s="13" t="s">
+      <c r="P26" s="17"/>
+      <c r="Q26" s="17"/>
+      <c r="R26" s="17"/>
+      <c r="S26" s="17"/>
+      <c r="T26" s="17"/>
+      <c r="U26" s="17"/>
+      <c r="V26" s="17"/>
+      <c r="W26" s="17"/>
+      <c r="X26" s="14"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1"/>
+      <c r="AB26" s="1"/>
+    </row>
+    <row r="27" spans="2:28" ht="6.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O27" s="12"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="14"/>
+    </row>
+    <row r="28" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L28" s="17"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="17"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="17"/>
+      <c r="Q28" s="17"/>
+      <c r="R28" s="17"/>
+      <c r="S28" s="17"/>
+      <c r="T28" s="1"/>
+      <c r="W28" s="17"/>
+      <c r="X28" s="17"/>
+      <c r="Y28" s="17"/>
+      <c r="Z28" s="17"/>
+      <c r="AA28" s="1"/>
+      <c r="AB28" s="1"/>
+    </row>
+    <row r="29" spans="2:28" ht="6.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K29" s="12"/>
+    </row>
+    <row r="30" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K30" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="K30" s="13"/>
-      <c r="L30" s="13"/>
-      <c r="N30" s="13" t="s">
+      <c r="L30" s="17"/>
+      <c r="M30" s="16"/>
+      <c r="O30" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="O30" s="13"/>
-      <c r="P30" s="13"/>
-      <c r="R30" s="13" t="s">
+      <c r="P30" s="17"/>
+      <c r="Q30" s="16"/>
+      <c r="S30" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="S30" s="13"/>
-      <c r="T30" s="13"/>
-      <c r="V30" s="13" t="s">
+      <c r="T30" s="17"/>
+      <c r="V30" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="W30" s="13"/>
-      <c r="X30" s="13"/>
-      <c r="Z30" s="13" t="s">
+      <c r="W30" s="17"/>
+      <c r="X30" s="14"/>
+      <c r="Z30" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="AA30" s="13"/>
-      <c r="AB30" s="13"/>
-    </row>
-    <row r="31" spans="2:28" ht="5.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="J31" s="16"/>
-      <c r="L31" s="15"/>
-      <c r="N31" s="16"/>
-      <c r="P31" s="15"/>
-      <c r="R31" s="14"/>
-      <c r="T31" s="15"/>
-      <c r="V31" s="16"/>
-      <c r="X31" s="15"/>
-      <c r="Z31" s="16"/>
-      <c r="AB31" s="15"/>
-    </row>
-    <row r="32" spans="2:28" x14ac:dyDescent="0.55000000000000004">
-      <c r="J32" s="7" t="s">
+      <c r="AA30" s="17"/>
+      <c r="AB30" s="14"/>
+    </row>
+    <row r="31" spans="2:28" ht="5.65" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K31" s="10"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="14"/>
+      <c r="O31" s="10"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="14"/>
+      <c r="S31" s="8"/>
+      <c r="T31" s="9"/>
+      <c r="V31" s="10"/>
+      <c r="W31" s="9"/>
+      <c r="X31" s="14"/>
+      <c r="Z31" s="10"/>
+      <c r="AA31" s="9"/>
+      <c r="AB31" s="14"/>
+    </row>
+    <row r="32" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="K32" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="L32" s="19" t="s">
+      <c r="L32" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="N32" s="7" t="s">
+      <c r="M32" s="13"/>
+      <c r="O32" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="P32" s="19" t="s">
+      <c r="P32" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="R32" s="7" t="s">
+      <c r="Q32" s="13"/>
+      <c r="S32" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="T32" s="19" t="s">
+      <c r="T32" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="V32" s="7" t="s">
+      <c r="V32" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="X32" s="19" t="s">
+      <c r="W32" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="Z32" s="7" t="s">
+      <c r="X32" s="13"/>
+      <c r="Z32" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AB32" s="19" t="s">
+      <c r="AA32" s="13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="15:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="O34" s="12"/>
-    </row>
-    <row r="36" spans="15:20" x14ac:dyDescent="0.55000000000000004">
-      <c r="T36" s="12"/>
+      <c r="AB32" s="13"/>
+    </row>
+    <row r="36" spans="9:31" x14ac:dyDescent="0.25">
+      <c r="N36" s="14"/>
+      <c r="O36" s="14"/>
+      <c r="P36" s="14"/>
+      <c r="Q36" s="14"/>
+      <c r="R36" s="14"/>
+      <c r="S36" s="14"/>
+      <c r="T36" s="15"/>
+      <c r="U36" s="14"/>
+      <c r="V36" s="14"/>
+      <c r="W36" s="14"/>
+      <c r="X36" s="14"/>
+      <c r="Y36" s="14"/>
+      <c r="Z36" s="14"/>
+    </row>
+    <row r="37" spans="9:31" x14ac:dyDescent="0.25">
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="16"/>
+      <c r="Q37" s="16"/>
+      <c r="R37" s="16"/>
+      <c r="S37" s="16"/>
+      <c r="T37" s="16"/>
+      <c r="U37" s="16"/>
+      <c r="V37" s="16"/>
+      <c r="W37" s="16"/>
+      <c r="X37" s="14"/>
+      <c r="Y37" s="16"/>
+      <c r="Z37" s="16"/>
+      <c r="AA37" s="1"/>
+      <c r="AB37" s="1"/>
+    </row>
+    <row r="38" spans="9:31" x14ac:dyDescent="0.25">
+      <c r="N38" s="14"/>
+      <c r="O38" s="14"/>
+      <c r="P38" s="14"/>
+      <c r="Q38" s="14"/>
+      <c r="R38" s="14"/>
+      <c r="S38" s="14"/>
+      <c r="T38" s="14"/>
+      <c r="U38" s="14"/>
+      <c r="V38" s="14"/>
+      <c r="W38" s="14"/>
+      <c r="X38" s="14"/>
+      <c r="Y38" s="14"/>
+      <c r="Z38" s="14"/>
+    </row>
+    <row r="39" spans="9:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="L39" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="M39" s="18"/>
+      <c r="N39" s="18"/>
+      <c r="O39" s="18"/>
+      <c r="P39" s="18"/>
+      <c r="Q39" s="18"/>
+      <c r="R39" s="18"/>
+      <c r="S39" s="18"/>
+      <c r="T39" s="1"/>
+      <c r="W39" s="16"/>
+      <c r="X39" s="16"/>
+      <c r="Y39" s="16"/>
+      <c r="Z39" s="16"/>
+      <c r="AA39" s="1"/>
+      <c r="AB39" s="1"/>
+    </row>
+    <row r="40" spans="9:31" x14ac:dyDescent="0.25">
+      <c r="K40" s="12"/>
+      <c r="P40" s="10"/>
+      <c r="T40" s="11"/>
+      <c r="V40" s="14"/>
+      <c r="W40" s="14"/>
+      <c r="X40" s="14"/>
+      <c r="Y40" s="14"/>
+      <c r="Z40" s="14"/>
+      <c r="AA40" s="14"/>
+      <c r="AB40" s="14"/>
+    </row>
+    <row r="41" spans="9:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K41" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="L41" s="18"/>
+      <c r="M41" s="16"/>
+      <c r="O41" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="P41" s="18"/>
+      <c r="Q41" s="16"/>
+      <c r="S41" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="T41" s="18"/>
+      <c r="V41" s="16"/>
+      <c r="W41" s="16"/>
+      <c r="X41" s="14"/>
+      <c r="Y41" s="14"/>
+      <c r="Z41" s="16"/>
+      <c r="AA41" s="16"/>
+      <c r="AB41" s="14"/>
+    </row>
+    <row r="42" spans="9:31" x14ac:dyDescent="0.25">
+      <c r="K42" s="10"/>
+      <c r="L42" s="9"/>
+      <c r="M42" s="14"/>
+      <c r="O42" s="10"/>
+      <c r="P42" s="9"/>
+      <c r="Q42" s="14"/>
+      <c r="S42" s="10"/>
+      <c r="T42" s="9"/>
+      <c r="V42" s="14"/>
+      <c r="W42" s="14"/>
+      <c r="X42" s="14"/>
+      <c r="Y42" s="14"/>
+      <c r="Z42" s="14"/>
+      <c r="AA42" s="14"/>
+      <c r="AB42" s="14"/>
+    </row>
+    <row r="43" spans="9:31" x14ac:dyDescent="0.25">
+      <c r="I43" s="1"/>
+      <c r="J43" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="K43" s="19"/>
+      <c r="L43" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="M43" s="19"/>
+      <c r="N43" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="O43" s="19"/>
+      <c r="P43" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q43" s="19"/>
+      <c r="R43" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="S43" s="1"/>
+      <c r="T43" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="U43" s="19"/>
+      <c r="V43" s="5"/>
+      <c r="W43" s="13"/>
+      <c r="X43" s="13"/>
+      <c r="Z43" s="5"/>
+      <c r="AA43" s="13"/>
+      <c r="AB43" s="13"/>
+    </row>
+    <row r="45" spans="9:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="W45" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="X45" s="18"/>
+      <c r="Y45" s="18"/>
+      <c r="Z45" s="18"/>
+      <c r="AA45" s="18"/>
+      <c r="AB45" s="18"/>
+      <c r="AC45" s="18"/>
+      <c r="AD45" s="18"/>
+      <c r="AE45" s="1"/>
+    </row>
+    <row r="46" spans="9:31" x14ac:dyDescent="0.25">
+      <c r="V46" s="12"/>
+      <c r="AA46" s="10"/>
+      <c r="AE46" s="11"/>
+    </row>
+    <row r="47" spans="9:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="V47" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="W47" s="18"/>
+      <c r="X47" s="14"/>
+      <c r="Z47" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="AA47" s="18"/>
+      <c r="AB47" s="14"/>
+      <c r="AD47" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE47" s="18"/>
+    </row>
+    <row r="48" spans="9:31" x14ac:dyDescent="0.25">
+      <c r="V48" s="10"/>
+      <c r="W48" s="9"/>
+      <c r="X48" s="14"/>
+      <c r="Z48" s="10"/>
+      <c r="AA48" s="9"/>
+      <c r="AB48" s="14"/>
+      <c r="AD48" s="10"/>
+      <c r="AE48" s="9"/>
+    </row>
+    <row r="49" spans="21:32" x14ac:dyDescent="0.25">
+      <c r="U49" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="V49" s="19"/>
+      <c r="W49" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="X49" s="19"/>
+      <c r="Y49" s="19" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z49" s="19"/>
+      <c r="AA49" s="19" t="s">
+        <v>6</v>
+      </c>
+      <c r="AB49" s="19"/>
+      <c r="AC49" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="AD49" s="19"/>
+      <c r="AE49" s="19" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF49" s="19"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="W28:Z28"/>
-    <mergeCell ref="J30:L30"/>
-    <mergeCell ref="N30:P30"/>
-    <mergeCell ref="R30:T30"/>
-    <mergeCell ref="V30:X30"/>
-    <mergeCell ref="Z30:AB30"/>
-    <mergeCell ref="N26:X26"/>
-    <mergeCell ref="K28:R28"/>
+  <mergeCells count="27">
+    <mergeCell ref="L39:S39"/>
     <mergeCell ref="D5:D15"/>
     <mergeCell ref="B5:B23"/>
     <mergeCell ref="F9:F11"/>
@@ -967,6 +1195,24 @@
     <mergeCell ref="F21:F23"/>
     <mergeCell ref="D17:D23"/>
     <mergeCell ref="F5:F7"/>
+    <mergeCell ref="AD47:AE47"/>
+    <mergeCell ref="AC49:AD49"/>
+    <mergeCell ref="AE49:AF49"/>
+    <mergeCell ref="AA49:AB49"/>
+    <mergeCell ref="V47:W47"/>
+    <mergeCell ref="Z47:AA47"/>
+    <mergeCell ref="Y49:Z49"/>
+    <mergeCell ref="U49:V49"/>
+    <mergeCell ref="W49:X49"/>
+    <mergeCell ref="W45:AD45"/>
+    <mergeCell ref="J43:K43"/>
+    <mergeCell ref="L43:M43"/>
+    <mergeCell ref="K41:L41"/>
+    <mergeCell ref="O41:P41"/>
+    <mergeCell ref="N43:O43"/>
+    <mergeCell ref="P43:Q43"/>
+    <mergeCell ref="S41:T41"/>
+    <mergeCell ref="T43:U43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>